<commit_message>
CCB July 2024 Update: IHME tab revamp; Enhanced Life Course tabs; City LHJs added to Hosp/ED tabs; Improved icd10-ccb image; manifest file removed
</commit_message>
<xml_diff>
--- a/myCCB/Standards/raceLink.xlsx
+++ b/myCCB/Standards/raceLink.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\Standards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\Standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A8A64F-595F-4942-95F1-6E55C9382C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -261,7 +262,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -587,25 +588,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="44.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="61.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -613,16 +616,16 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F1" t="s">
         <v>24</v>
@@ -643,13 +646,13 @@
         <v>44</v>
       </c>
       <c r="L1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="M1" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="N1" t="s">
-        <v>75</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -657,16 +660,16 @@
         <v>62</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>0</v>
@@ -686,14 +689,14 @@
       <c r="K2" t="s">
         <v>47</v>
       </c>
-      <c r="L2" t="s">
-        <v>59</v>
-      </c>
-      <c r="M2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="N2" t="s">
+      <c r="M2" t="s">
         <v>70</v>
+      </c>
+      <c r="N2">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -701,16 +704,16 @@
         <v>30</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>2</v>
+      <c r="E3" t="s">
+        <v>57</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -731,13 +734,13 @@
         <v>46</v>
       </c>
       <c r="L3" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="M3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" t="s">
         <v>69</v>
+      </c>
+      <c r="N3">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -745,16 +748,16 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
       </c>
       <c r="F4" t="s">
         <v>1</v>
@@ -775,13 +778,13 @@
         <v>45</v>
       </c>
       <c r="L4" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>1</v>
-      </c>
-      <c r="N4" t="s">
         <v>71</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -789,16 +792,16 @@
         <v>36</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
@@ -819,27 +822,27 @@
         <v>49</v>
       </c>
       <c r="L5" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="M5" t="s">
-        <v>15</v>
-      </c>
-      <c r="N5" t="s">
         <v>73</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>63</v>
       </c>
-      <c r="B6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -860,13 +863,13 @@
         <v>50</v>
       </c>
       <c r="L6" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="M6" t="s">
-        <v>67</v>
-      </c>
-      <c r="N6" t="s">
         <v>72</v>
+      </c>
+      <c r="N6">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -874,16 +877,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>56</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -904,27 +907,27 @@
         <v>48</v>
       </c>
       <c r="L7" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="M7" t="s">
-        <v>10</v>
-      </c>
-      <c r="N7" t="s">
         <v>68</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>64</v>
       </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="D8">
+      <c r="C8">
         <v>7</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
@@ -945,13 +948,13 @@
         <v>51</v>
       </c>
       <c r="L8" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="M8" t="s">
-        <v>12</v>
-      </c>
-      <c r="N8" t="s">
         <v>74</v>
+      </c>
+      <c r="N8">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -959,15 +962,12 @@
         <v>5</v>
       </c>
       <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
         <v>8</v>
       </c>
-      <c r="C9">
-        <v>6</v>
-      </c>
-      <c r="D9">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F9" t="s">
@@ -979,8 +979,11 @@
       <c r="J9" t="s">
         <v>40</v>
       </c>
-      <c r="M9" t="s">
+      <c r="L9" t="s">
         <v>5</v>
+      </c>
+      <c r="N9">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -988,15 +991,12 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F10" t="s">
@@ -1008,8 +1008,11 @@
       <c r="J10" t="s">
         <v>39</v>
       </c>
-      <c r="M10" t="s">
-        <v>6</v>
+      <c r="L10" t="s">
+        <v>6</v>
+      </c>
+      <c r="N10">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1022,7 +1025,7 @@
       <c r="J11" t="s">
         <v>43</v>
       </c>
-      <c r="M11" t="s">
+      <c r="L11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1036,7 +1039,7 @@
       <c r="K12" t="s">
         <v>52</v>
       </c>
-      <c r="M12" t="s">
+      <c r="L12" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1047,7 +1050,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>